<commit_message>
EVERLINO SUNAT FEBRERO 14.02
</commit_message>
<xml_diff>
--- a/EVERLINO SUNAT.xlsx
+++ b/EVERLINO SUNAT.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lutay\Downloads\DIRECTV\TERRAMOVE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lutay\Downloads\DIRECTV\SUNAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D3F656-8609-45F3-BB6C-333804DC8C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5768AF13-460E-4CBB-A68E-EC8C9355BA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{09F33025-CD1B-49C8-89D2-345291A41180}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{09F33025-CD1B-49C8-89D2-345291A41180}"/>
   </bookViews>
   <sheets>
     <sheet name="+++" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="R.VENTAS" sheetId="4" r:id="rId2"/>
     <sheet name="R.COMPRAS" sheetId="3" r:id="rId3"/>
     <sheet name="Enero-2022" sheetId="2" state="hidden" r:id="rId4"/>
-    <sheet name="LIQ.IMPUESTOS 01.2022" sheetId="5" r:id="rId5"/>
+    <sheet name="LIQ.IMPUESTOS 02.2022" sheetId="5" r:id="rId5"/>
     <sheet name="CRONOGRAMA" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="103">
   <si>
     <t>DECLARACION ANUAL DE IR</t>
   </si>
@@ -203,15 +203,9 @@
     <t>BASE IMPONIBLE</t>
   </si>
   <si>
-    <t>E001</t>
-  </si>
-  <si>
     <t>RUC</t>
   </si>
   <si>
-    <t>GRUPO JAZIEL S.A.C</t>
-  </si>
-  <si>
     <t>IMPORTE TOTAL</t>
   </si>
   <si>
@@ -287,28 +281,127 @@
     <t>CREDITO FISCAL A FAVOR</t>
   </si>
   <si>
-    <t>F36T</t>
-  </si>
-  <si>
-    <t>COESTI S.A.</t>
-  </si>
-  <si>
-    <t>LIMA EXPRESA S.A.C</t>
-  </si>
-  <si>
-    <t>F155</t>
-  </si>
-  <si>
-    <t>FH04</t>
-  </si>
-  <si>
-    <t>INTERBANK</t>
-  </si>
-  <si>
-    <t>F214</t>
-  </si>
-  <si>
-    <t>RUTAS DE LIMA SAC</t>
+    <t>F001</t>
+  </si>
+  <si>
+    <t>NEGOCIACIONES ALEPI S.A.C</t>
+  </si>
+  <si>
+    <t>F008</t>
+  </si>
+  <si>
+    <t>0000020696</t>
+  </si>
+  <si>
+    <t>JAARSOM E.I.R.L</t>
+  </si>
+  <si>
+    <t>00021387</t>
+  </si>
+  <si>
+    <t>FAPIGRIFOS S.A.C</t>
+  </si>
+  <si>
+    <t>F006</t>
+  </si>
+  <si>
+    <t>0053209</t>
+  </si>
+  <si>
+    <t>MONTE EVEREST S.A.C</t>
+  </si>
+  <si>
+    <t>SERVICENTRO CERRO AZUL E.I.R.L</t>
+  </si>
+  <si>
+    <t>00016079</t>
+  </si>
+  <si>
+    <t>00001264</t>
+  </si>
+  <si>
+    <t>GROUP MACKRE E.I.R.L</t>
+  </si>
+  <si>
+    <t>F203</t>
+  </si>
+  <si>
+    <t>00800086</t>
+  </si>
+  <si>
+    <t>CONCESIONARIA VIAL DEL PERU S.A</t>
+  </si>
+  <si>
+    <t>F608</t>
+  </si>
+  <si>
+    <t>00247882</t>
+  </si>
+  <si>
+    <t>RUTAS DE LIMA S.A.C</t>
+  </si>
+  <si>
+    <t>REPSOL COMERCIAL S.A.C</t>
+  </si>
+  <si>
+    <t>F569</t>
+  </si>
+  <si>
+    <t>00053977</t>
+  </si>
+  <si>
+    <t>00017132</t>
+  </si>
+  <si>
+    <t>F114</t>
+  </si>
+  <si>
+    <t>FFF1</t>
+  </si>
+  <si>
+    <t>11734</t>
+  </si>
+  <si>
+    <t>ROMIS E.I.R.L</t>
+  </si>
+  <si>
+    <t>FS56</t>
+  </si>
+  <si>
+    <t>00004281</t>
+  </si>
+  <si>
+    <t>SERVICENTROS PLAZA S.A.C.</t>
+  </si>
+  <si>
+    <t>CLINICA INTERNACIONAL</t>
+  </si>
+  <si>
+    <t>FC10</t>
+  </si>
+  <si>
+    <t>00000458</t>
+  </si>
+  <si>
+    <t>CIERTO ROJAS BERLINA</t>
+  </si>
+  <si>
+    <t>F004</t>
+  </si>
+  <si>
+    <t>00052592</t>
+  </si>
+  <si>
+    <t>F106</t>
+  </si>
+  <si>
+    <t>00242084</t>
+  </si>
+  <si>
+    <t>F568</t>
+  </si>
+  <si>
+    <t>00087004</t>
   </si>
 </sst>
 </file>
@@ -1143,7 +1236,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1390,6 +1483,12 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1887,7 +1986,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1897,7 +1996,7 @@
     <col min="5" max="5" width="22.44140625" style="16" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" style="16" customWidth="1"/>
     <col min="7" max="7" width="16" style="16" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" style="16" customWidth="1"/>
+    <col min="8" max="8" width="26.109375" style="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.44140625" style="16" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11.5546875" style="16"/>
   </cols>
@@ -1907,7 +2006,7 @@
         <v>31</v>
       </c>
       <c r="B1" s="87" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C1" s="89" t="s">
         <v>33</v>
@@ -1928,7 +2027,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="79" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1973,37 +2072,23 @@
       <c r="A4" s="40">
         <v>1</v>
       </c>
-      <c r="B4" s="26">
-        <v>44592</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="27">
-        <v>3</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="28">
-        <v>20608130668</v>
-      </c>
-      <c r="H4" s="28" t="s">
-        <v>38</v>
-      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
       <c r="I4" s="29">
         <f>K4/1.18</f>
-        <v>3905.0847457627119</v>
+        <v>0</v>
       </c>
       <c r="J4" s="30">
         <f>I4*0.18</f>
-        <v>702.91525423728808</v>
+        <v>0</v>
       </c>
       <c r="K4" s="41">
-        <v>4608</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2013,7 +2098,7 @@
       <c r="B5" s="26"/>
       <c r="C5" s="25"/>
       <c r="D5" s="25"/>
-      <c r="E5" s="27"/>
+      <c r="E5" s="107"/>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
       <c r="H5" s="28"/>
@@ -2036,7 +2121,7 @@
       <c r="B6" s="26"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
-      <c r="E6" s="27"/>
+      <c r="E6" s="107"/>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
@@ -2059,7 +2144,7 @@
       <c r="B7" s="26"/>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
-      <c r="E7" s="27"/>
+      <c r="E7" s="107"/>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
@@ -2083,7 +2168,7 @@
       <c r="B8" s="26"/>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
-      <c r="E8" s="27"/>
+      <c r="E8" s="107"/>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
@@ -2106,7 +2191,7 @@
       <c r="B9" s="26"/>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
-      <c r="E9" s="27"/>
+      <c r="E9" s="107"/>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
@@ -2129,7 +2214,7 @@
       <c r="B10" s="26"/>
       <c r="C10" s="25"/>
       <c r="D10" s="25"/>
-      <c r="E10" s="27"/>
+      <c r="E10" s="107"/>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
@@ -2152,7 +2237,7 @@
       <c r="B11" s="26"/>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
-      <c r="E11" s="27"/>
+      <c r="E11" s="107"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
@@ -2175,7 +2260,7 @@
       <c r="B12" s="26"/>
       <c r="C12" s="25"/>
       <c r="D12" s="25"/>
-      <c r="E12" s="27"/>
+      <c r="E12" s="107"/>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
@@ -2198,7 +2283,7 @@
       <c r="B13" s="26"/>
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
-      <c r="E13" s="27"/>
+      <c r="E13" s="107"/>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
@@ -2221,7 +2306,7 @@
       <c r="B14" s="26"/>
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="27"/>
+      <c r="E14" s="107"/>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
@@ -2244,7 +2329,7 @@
       <c r="B15" s="26"/>
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
-      <c r="E15" s="27"/>
+      <c r="E15" s="107"/>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>
@@ -2267,7 +2352,7 @@
       <c r="B16" s="26"/>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
-      <c r="E16" s="27"/>
+      <c r="E16" s="107"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
@@ -2290,7 +2375,7 @@
       <c r="B17" s="26"/>
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="27"/>
+      <c r="E17" s="107"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
@@ -2313,7 +2398,7 @@
       <c r="B18" s="26"/>
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
-      <c r="E18" s="27"/>
+      <c r="E18" s="107"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
       <c r="H18" s="28"/>
@@ -2336,7 +2421,7 @@
       <c r="B19" s="26"/>
       <c r="C19" s="25"/>
       <c r="D19" s="25"/>
-      <c r="E19" s="27"/>
+      <c r="E19" s="107"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
@@ -2359,7 +2444,7 @@
       <c r="B20" s="26"/>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
-      <c r="E20" s="27"/>
+      <c r="E20" s="107"/>
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
@@ -2382,7 +2467,7 @@
       <c r="B21" s="26"/>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
-      <c r="E21" s="27"/>
+      <c r="E21" s="107"/>
       <c r="F21" s="28"/>
       <c r="G21" s="28"/>
       <c r="H21" s="28"/>
@@ -2405,7 +2490,7 @@
       <c r="B22" s="26"/>
       <c r="C22" s="25"/>
       <c r="D22" s="25"/>
-      <c r="E22" s="27"/>
+      <c r="E22" s="107"/>
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
@@ -2428,7 +2513,7 @@
       <c r="B23" s="26"/>
       <c r="C23" s="25"/>
       <c r="D23" s="25"/>
-      <c r="E23" s="27"/>
+      <c r="E23" s="107"/>
       <c r="F23" s="28"/>
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
@@ -2451,7 +2536,7 @@
       <c r="B24" s="26"/>
       <c r="C24" s="25"/>
       <c r="D24" s="25"/>
-      <c r="E24" s="27"/>
+      <c r="E24" s="107"/>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
@@ -2474,7 +2559,7 @@
       <c r="B25" s="26"/>
       <c r="C25" s="25"/>
       <c r="D25" s="25"/>
-      <c r="E25" s="27"/>
+      <c r="E25" s="107"/>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
       <c r="H25" s="28"/>
@@ -2497,7 +2582,7 @@
       <c r="B26" s="32"/>
       <c r="C26" s="31"/>
       <c r="D26" s="31"/>
-      <c r="E26" s="33"/>
+      <c r="E26" s="108"/>
       <c r="F26" s="34"/>
       <c r="G26" s="34"/>
       <c r="H26" s="34"/>
@@ -2526,15 +2611,15 @@
       <c r="H27" s="75"/>
       <c r="I27" s="37">
         <f>SUM(I4:I26)</f>
-        <v>3905.0847457627119</v>
+        <v>0</v>
       </c>
       <c r="J27" s="38">
         <f>SUM(J4:J26)</f>
-        <v>702.91525423728808</v>
+        <v>0</v>
       </c>
       <c r="K27" s="39">
         <f>SUM(K4:K26)</f>
-        <v>4608</v>
+        <v>0</v>
       </c>
       <c r="L27" s="61"/>
     </row>
@@ -2566,8 +2651,8 @@
   </sheetPr>
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -2587,7 +2672,7 @@
         <v>31</v>
       </c>
       <c r="B1" s="87" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C1" s="89" t="s">
         <v>33</v>
@@ -2608,7 +2693,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="79" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -2654,36 +2739,36 @@
         <v>1</v>
       </c>
       <c r="B4" s="26">
-        <v>44591</v>
+        <v>44598</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="27">
-        <v>30966</v>
+        <v>62</v>
+      </c>
+      <c r="E4" s="107">
+        <v>10575</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" s="28">
-        <v>20127765279</v>
+        <v>20494629055</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I4" s="29">
         <f>K4/1.18</f>
-        <v>42.372881355932208</v>
+        <v>61.779661016949163</v>
       </c>
       <c r="J4" s="29">
         <f>I4*0.18</f>
-        <v>7.6271186440677967</v>
+        <v>11.120338983050848</v>
       </c>
       <c r="K4" s="65">
-        <v>50</v>
+        <v>72.900000000000006</v>
       </c>
       <c r="L4" s="64"/>
     </row>
@@ -2692,36 +2777,36 @@
         <v>2</v>
       </c>
       <c r="B5" s="26">
-        <v>44591</v>
+        <v>44599</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="27">
-        <v>2813690</v>
+        <v>64</v>
+      </c>
+      <c r="E5" s="107" t="s">
+        <v>65</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5" s="28">
-        <v>20523621212</v>
+        <v>20534249960</v>
       </c>
       <c r="H5" s="28" t="s">
         <v>66</v>
       </c>
       <c r="I5" s="29">
         <f t="shared" ref="I5:I26" si="0">K5/1.18</f>
-        <v>5.0000000000000009</v>
+        <v>127.11864406779662</v>
       </c>
       <c r="J5" s="30">
         <f t="shared" ref="J5:J26" si="1">I5*0.18</f>
-        <v>0.90000000000000013</v>
+        <v>22.881355932203391</v>
       </c>
       <c r="K5" s="41">
-        <v>5.9</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2732,32 +2817,33 @@
         <v>44594</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D6" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="107" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="28">
+        <v>20601770475</v>
+      </c>
+      <c r="H6" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="27">
-        <v>437726</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="28">
-        <v>20100053455</v>
-      </c>
-      <c r="H6" s="28" t="s">
-        <v>69</v>
-      </c>
       <c r="I6" s="29">
-        <f>K6</f>
-        <v>1681.76</v>
+        <f t="shared" si="0"/>
+        <v>59.322033898305087</v>
       </c>
       <c r="J6" s="30">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>10.677966101694915</v>
       </c>
       <c r="K6" s="41">
-        <v>1681.76</v>
+        <v>70</v>
       </c>
       <c r="M6" s="64"/>
     </row>
@@ -2766,312 +2852,480 @@
         <v>4</v>
       </c>
       <c r="B7" s="26">
-        <v>44591</v>
+        <v>44604</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="107" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="27">
-        <v>1540975</v>
-      </c>
       <c r="F7" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="28">
-        <v>20550372640</v>
+        <v>20511193045</v>
       </c>
       <c r="H7" s="28" t="s">
         <v>71</v>
       </c>
       <c r="I7" s="29">
         <f t="shared" si="0"/>
-        <v>4.6610169491525424</v>
+        <v>42.372881355932208</v>
       </c>
       <c r="J7" s="30">
         <f t="shared" si="1"/>
-        <v>0.83898305084745761</v>
+        <v>7.6271186440677967</v>
       </c>
       <c r="K7" s="41">
-        <v>5.5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="40">
         <v>5</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
+      <c r="B8" s="26">
+        <v>44604</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="107" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="28">
+        <v>20602334211</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>72</v>
+      </c>
       <c r="I8" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42.372881355932208</v>
       </c>
       <c r="J8" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.6271186440677967</v>
       </c>
       <c r="K8" s="41">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="40">
         <v>6</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
+      <c r="B9" s="26">
+        <v>44603</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="107" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="28">
+        <v>20602756921</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>75</v>
+      </c>
       <c r="I9" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>84.745762711864415</v>
       </c>
       <c r="J9" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15.254237288135593</v>
       </c>
       <c r="K9" s="41">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="40">
         <v>7</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
+      <c r="B10" s="26">
+        <v>44604</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="107" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="28">
+        <v>20511465061</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>78</v>
+      </c>
       <c r="I10" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13.389830508474578</v>
       </c>
       <c r="J10" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.4101694915254241</v>
       </c>
       <c r="K10" s="41">
-        <v>0</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>8</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
+      <c r="B11" s="26">
+        <v>44604</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="107" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="28">
+        <v>20550372640</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>81</v>
+      </c>
       <c r="I11" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.6610169491525424</v>
       </c>
       <c r="J11" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.83898305084745761</v>
       </c>
       <c r="K11" s="41">
-        <v>0</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
         <v>9</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
+      <c r="B12" s="26">
+        <v>44605</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="107" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="28">
+        <v>20503840121</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>82</v>
+      </c>
       <c r="I12" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>173.47457627118644</v>
       </c>
       <c r="J12" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>31.225423728813556</v>
       </c>
       <c r="K12" s="41">
-        <v>0</v>
+        <v>204.7</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="40">
         <v>10</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
+      <c r="B13" s="26">
+        <v>44605</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="107" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="28">
+        <v>20511465061</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>78</v>
+      </c>
       <c r="I13" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13.389830508474578</v>
       </c>
       <c r="J13" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.4101694915254241</v>
       </c>
       <c r="K13" s="41">
-        <v>0</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>11</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
+      <c r="B14" s="26">
+        <v>44598</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="107" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="28">
+        <v>20511849048</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>89</v>
+      </c>
       <c r="I14" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13.254237288135595</v>
       </c>
       <c r="J14" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.3857627118644071</v>
       </c>
       <c r="K14" s="41">
-        <v>0</v>
+        <v>15.64</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
         <v>12</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
+      <c r="B15" s="26">
+        <v>44598</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="107" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="28">
+        <v>20452262399</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>92</v>
+      </c>
       <c r="I15" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>97.440677966101703</v>
       </c>
       <c r="J15" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>17.539322033898305</v>
       </c>
       <c r="K15" s="41">
-        <v>0</v>
+        <v>114.98</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="40">
         <v>13</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
+      <c r="B16" s="26">
+        <v>44606</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="107" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="28">
+        <v>20100054184</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>93</v>
+      </c>
       <c r="I16" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>41.872881355932201</v>
       </c>
       <c r="J16" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.537118644067796</v>
       </c>
       <c r="K16" s="41">
-        <v>0</v>
+        <v>49.41</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="40">
         <v>14</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
+      <c r="B17" s="26">
+        <v>44597</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="107" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="28">
+        <v>10225180721</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>96</v>
+      </c>
       <c r="I17" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>84.745762711864415</v>
       </c>
       <c r="J17" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15.254237288135593</v>
       </c>
       <c r="K17" s="41">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="40">
         <v>15</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
+      <c r="B18" s="26">
+        <v>44598</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="107" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="28">
+        <v>20511465061</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>78</v>
+      </c>
       <c r="I18" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13.389830508474578</v>
       </c>
       <c r="J18" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.4101694915254241</v>
       </c>
       <c r="K18" s="41">
-        <v>0</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="40">
         <v>16</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
+      <c r="B19" s="26">
+        <v>44598</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="107" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="28">
+        <v>20503840121</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>82</v>
+      </c>
       <c r="I19" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100.92372881355934</v>
       </c>
       <c r="J19" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>18.166271186440678</v>
       </c>
       <c r="K19" s="41">
-        <v>0</v>
+        <v>119.09</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3248,15 +3502,15 @@
       <c r="H27" s="75"/>
       <c r="I27" s="37">
         <f>SUM(I4:I26)</f>
-        <v>1733.7938983050847</v>
+        <v>974.25423728813587</v>
       </c>
       <c r="J27" s="38">
         <f>SUM(J4:J26)</f>
-        <v>9.3661016949152547</v>
+        <v>175.36576271186439</v>
       </c>
       <c r="K27" s="39">
         <f>SUM(K4:K26)</f>
-        <v>1743.16</v>
+        <v>1149.6199999999999</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -3264,6 +3518,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A27:H27"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="J1:J3"/>
     <mergeCell ref="K1:K3"/>
@@ -3272,11 +3531,6 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A27:H27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3459,8 +3713,8 @@
   </sheetPr>
   <dimension ref="B1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3477,7 +3731,7 @@
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="97" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="98"/>
       <c r="D2" s="99"/>
@@ -3489,17 +3743,17 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="103" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="104"/>
       <c r="D5" s="105" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E5" s="106"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="103" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="104"/>
       <c r="D6" s="105">
@@ -3509,21 +3763,21 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="103" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" s="104"/>
       <c r="D7" s="105" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E7" s="106"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="103" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" s="104"/>
       <c r="D8" s="105" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E8" s="106"/>
     </row>
@@ -3541,7 +3795,7 @@
       <c r="B11" s="50"/>
       <c r="C11" s="51"/>
       <c r="D11" s="52" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E11" s="51"/>
       <c r="F11" s="51"/>
@@ -3561,7 +3815,7 @@
       <c r="B13" s="50"/>
       <c r="C13" s="51"/>
       <c r="D13" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>9</v>
@@ -3588,15 +3842,15 @@
       </c>
       <c r="D15" s="44">
         <f>'R.VENTAS'!$I$27</f>
-        <v>3905.0847457627119</v>
+        <v>0</v>
       </c>
       <c r="E15" s="45">
         <f>'R.VENTAS'!$J$27</f>
-        <v>702.91525423728808</v>
+        <v>0</v>
       </c>
       <c r="F15" s="46">
         <f>SUM(D15:E15)</f>
-        <v>4608</v>
+        <v>0</v>
       </c>
       <c r="G15" s="51"/>
       <c r="H15" s="53"/>
@@ -3617,15 +3871,15 @@
       </c>
       <c r="D17" s="44">
         <f>'R.COMPRAS'!$I$27</f>
-        <v>1733.7938983050847</v>
+        <v>974.25423728813587</v>
       </c>
       <c r="E17" s="45">
         <f>'R.COMPRAS'!$J$27</f>
-        <v>9.3661016949152547</v>
+        <v>175.36576271186439</v>
       </c>
       <c r="F17" s="45">
         <f>SUM(D17:E17)</f>
-        <v>1743.1599999999999</v>
+        <v>1149.6200000000003</v>
       </c>
       <c r="G17" s="51"/>
       <c r="H17" s="53"/>
@@ -3651,7 +3905,7 @@
     <row r="21" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="94" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22" s="95"/>
       <c r="D22" s="96"/>
@@ -3659,35 +3913,35 @@
     <row r="23" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E24" s="58" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J24" s="73"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F25" s="59" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G25" s="62">
         <f>E15-E17</f>
-        <v>693.54915254237278</v>
+        <v>-175.36576271186439</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F26" s="59" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G26" s="60">
         <f>IF(E15&lt;E17,E17-E15,0)</f>
-        <v>0</v>
+        <v>175.36576271186439</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F27" s="59" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G27" s="70">
         <f>IF(G26&gt;G25,0,G25-G26)</f>
-        <v>693.54915254237278</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -3701,7 +3955,7 @@
     <row r="31" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="32" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E32" s="58" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
@@ -3710,12 +3964,12 @@
       </c>
       <c r="G33" s="62">
         <f>$D$15</f>
-        <v>3905.0847457627119</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F34" s="59" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G34" s="66">
         <v>1.4999999999999999E-2</v>
@@ -3723,32 +3977,32 @@
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F35" s="59" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G35" s="60">
         <f>G33*G34</f>
-        <v>58.576271186440678</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F36" s="59" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G36" s="60"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F37" s="59" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G37" s="71">
         <f>G35-G36</f>
-        <v>58.576271186440678</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="39" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="94" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C39" s="95"/>
       <c r="D39" s="96"/>
@@ -3756,10 +4010,10 @@
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E41" s="67"/>
       <c r="F41" s="68" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G41" s="68" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H41" s="68" t="s">
         <v>10</v>
@@ -3767,36 +4021,36 @@
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E42" s="69" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F42" s="63">
         <f>$G$27</f>
-        <v>693.54915254237278</v>
+        <v>0</v>
       </c>
       <c r="G42" s="72"/>
       <c r="H42" s="63">
         <f>SUM(F42:G42)</f>
-        <v>693.54915254237278</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E43" s="69" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F43" s="63">
         <f>$G$37</f>
-        <v>58.576271186440678</v>
+        <v>0</v>
       </c>
       <c r="G43" s="72"/>
       <c r="H43" s="63">
         <f>SUM(F43:G43)</f>
-        <v>58.576271186440678</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F44" s="43">
         <f>SUM(F42:F43)</f>
-        <v>752.12542372881342</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3824,7 +4078,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
EVERLINO SUNAT MES DE FEBRERO
</commit_message>
<xml_diff>
--- a/EVERLINO SUNAT.xlsx
+++ b/EVERLINO SUNAT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lutay\Downloads\DIRECTV\SUNAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5768AF13-460E-4CBB-A68E-EC8C9355BA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260F96DB-D718-41F5-8912-1E4E332ADD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{09F33025-CD1B-49C8-89D2-345291A41180}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{09F33025-CD1B-49C8-89D2-345291A41180}"/>
   </bookViews>
   <sheets>
     <sheet name="+++" sheetId="1" state="hidden" r:id="rId1"/>
@@ -1385,6 +1385,12 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1483,12 +1489,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2002,71 +2002,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="90"/>
-      <c r="E1" s="87" t="s">
+      <c r="D1" s="92"/>
+      <c r="E1" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="91" t="s">
+      <c r="F1" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="89"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="87" t="s">
+      <c r="G1" s="91"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="76" t="s">
+      <c r="J1" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="K1" s="81" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="85"/>
-      <c r="B2" s="88"/>
-      <c r="C2" s="77" t="s">
+      <c r="A2" s="87"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="88"/>
-      <c r="F2" s="77" t="s">
+      <c r="E2" s="90"/>
+      <c r="F2" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="77"/>
-      <c r="H2" s="82" t="s">
+      <c r="G2" s="79"/>
+      <c r="H2" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="88"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="80"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="82"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="86"/>
-      <c r="B3" s="82"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="82"/>
+      <c r="A3" s="88"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="84"/>
       <c r="F3" s="24" t="s">
         <v>30</v>
       </c>
       <c r="G3" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="83"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="81"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="83"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="40">
@@ -2075,7 +2075,7 @@
       <c r="B4" s="26"/>
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
-      <c r="E4" s="107"/>
+      <c r="E4" s="74"/>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
       <c r="H4" s="28"/>
@@ -2098,7 +2098,7 @@
       <c r="B5" s="26"/>
       <c r="C5" s="25"/>
       <c r="D5" s="25"/>
-      <c r="E5" s="107"/>
+      <c r="E5" s="74"/>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
       <c r="H5" s="28"/>
@@ -2121,7 +2121,7 @@
       <c r="B6" s="26"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
-      <c r="E6" s="107"/>
+      <c r="E6" s="74"/>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
@@ -2144,7 +2144,7 @@
       <c r="B7" s="26"/>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
-      <c r="E7" s="107"/>
+      <c r="E7" s="74"/>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
@@ -2168,7 +2168,7 @@
       <c r="B8" s="26"/>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
-      <c r="E8" s="107"/>
+      <c r="E8" s="74"/>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
@@ -2191,7 +2191,7 @@
       <c r="B9" s="26"/>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
-      <c r="E9" s="107"/>
+      <c r="E9" s="74"/>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
@@ -2214,7 +2214,7 @@
       <c r="B10" s="26"/>
       <c r="C10" s="25"/>
       <c r="D10" s="25"/>
-      <c r="E10" s="107"/>
+      <c r="E10" s="74"/>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
@@ -2237,7 +2237,7 @@
       <c r="B11" s="26"/>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
-      <c r="E11" s="107"/>
+      <c r="E11" s="74"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
@@ -2260,7 +2260,7 @@
       <c r="B12" s="26"/>
       <c r="C12" s="25"/>
       <c r="D12" s="25"/>
-      <c r="E12" s="107"/>
+      <c r="E12" s="74"/>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
@@ -2283,7 +2283,7 @@
       <c r="B13" s="26"/>
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
-      <c r="E13" s="107"/>
+      <c r="E13" s="74"/>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
@@ -2306,7 +2306,7 @@
       <c r="B14" s="26"/>
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="107"/>
+      <c r="E14" s="74"/>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
@@ -2329,7 +2329,7 @@
       <c r="B15" s="26"/>
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
-      <c r="E15" s="107"/>
+      <c r="E15" s="74"/>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>
@@ -2352,7 +2352,7 @@
       <c r="B16" s="26"/>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
-      <c r="E16" s="107"/>
+      <c r="E16" s="74"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
@@ -2375,7 +2375,7 @@
       <c r="B17" s="26"/>
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="107"/>
+      <c r="E17" s="74"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
@@ -2398,7 +2398,7 @@
       <c r="B18" s="26"/>
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
-      <c r="E18" s="107"/>
+      <c r="E18" s="74"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
       <c r="H18" s="28"/>
@@ -2421,7 +2421,7 @@
       <c r="B19" s="26"/>
       <c r="C19" s="25"/>
       <c r="D19" s="25"/>
-      <c r="E19" s="107"/>
+      <c r="E19" s="74"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
@@ -2444,7 +2444,7 @@
       <c r="B20" s="26"/>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
-      <c r="E20" s="107"/>
+      <c r="E20" s="74"/>
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
@@ -2467,7 +2467,7 @@
       <c r="B21" s="26"/>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
-      <c r="E21" s="107"/>
+      <c r="E21" s="74"/>
       <c r="F21" s="28"/>
       <c r="G21" s="28"/>
       <c r="H21" s="28"/>
@@ -2490,7 +2490,7 @@
       <c r="B22" s="26"/>
       <c r="C22" s="25"/>
       <c r="D22" s="25"/>
-      <c r="E22" s="107"/>
+      <c r="E22" s="74"/>
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
@@ -2513,7 +2513,7 @@
       <c r="B23" s="26"/>
       <c r="C23" s="25"/>
       <c r="D23" s="25"/>
-      <c r="E23" s="107"/>
+      <c r="E23" s="74"/>
       <c r="F23" s="28"/>
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
@@ -2536,7 +2536,7 @@
       <c r="B24" s="26"/>
       <c r="C24" s="25"/>
       <c r="D24" s="25"/>
-      <c r="E24" s="107"/>
+      <c r="E24" s="74"/>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
@@ -2559,7 +2559,7 @@
       <c r="B25" s="26"/>
       <c r="C25" s="25"/>
       <c r="D25" s="25"/>
-      <c r="E25" s="107"/>
+      <c r="E25" s="74"/>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
       <c r="H25" s="28"/>
@@ -2582,7 +2582,7 @@
       <c r="B26" s="32"/>
       <c r="C26" s="31"/>
       <c r="D26" s="31"/>
-      <c r="E26" s="108"/>
+      <c r="E26" s="75"/>
       <c r="F26" s="34"/>
       <c r="G26" s="34"/>
       <c r="H26" s="34"/>
@@ -2599,16 +2599,16 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="74" t="s">
+      <c r="A27" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="75"/>
+      <c r="B27" s="77"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="77"/>
+      <c r="H27" s="77"/>
       <c r="I27" s="37">
         <f>SUM(I4:I26)</f>
         <v>0</v>
@@ -2651,8 +2651,8 @@
   </sheetPr>
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -2668,71 +2668,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="90"/>
-      <c r="E1" s="87" t="s">
+      <c r="D1" s="92"/>
+      <c r="E1" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="91" t="s">
+      <c r="F1" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="89"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="87" t="s">
+      <c r="G1" s="91"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="76" t="s">
+      <c r="J1" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="K1" s="81" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="85"/>
-      <c r="B2" s="88"/>
-      <c r="C2" s="77" t="s">
+      <c r="A2" s="87"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="88"/>
-      <c r="F2" s="77" t="s">
+      <c r="E2" s="90"/>
+      <c r="F2" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="77"/>
-      <c r="H2" s="82" t="s">
+      <c r="G2" s="79"/>
+      <c r="H2" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="88"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="80"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="82"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="85"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="88"/>
+      <c r="A3" s="87"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="90"/>
       <c r="F3" s="17" t="s">
         <v>30</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="92"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="80"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="82"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="40">
@@ -2747,7 +2747,7 @@
       <c r="D4" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="107">
+      <c r="E4" s="74">
         <v>10575</v>
       </c>
       <c r="F4" s="28" t="s">
@@ -2785,7 +2785,7 @@
       <c r="D5" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="107" t="s">
+      <c r="E5" s="74" t="s">
         <v>65</v>
       </c>
       <c r="F5" s="28" t="s">
@@ -2822,7 +2822,7 @@
       <c r="D6" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="107" t="s">
+      <c r="E6" s="74" t="s">
         <v>67</v>
       </c>
       <c r="F6" s="28" t="s">
@@ -2860,7 +2860,7 @@
       <c r="D7" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E7" s="107" t="s">
+      <c r="E7" s="74" t="s">
         <v>70</v>
       </c>
       <c r="F7" s="28" t="s">
@@ -2897,7 +2897,7 @@
       <c r="D8" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="107" t="s">
+      <c r="E8" s="74" t="s">
         <v>73</v>
       </c>
       <c r="F8" s="28" t="s">
@@ -2934,7 +2934,7 @@
       <c r="D9" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="107" t="s">
+      <c r="E9" s="74" t="s">
         <v>74</v>
       </c>
       <c r="F9" s="28" t="s">
@@ -2971,7 +2971,7 @@
       <c r="D10" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="107" t="s">
+      <c r="E10" s="74" t="s">
         <v>77</v>
       </c>
       <c r="F10" s="28" t="s">
@@ -3008,7 +3008,7 @@
       <c r="D11" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="107" t="s">
+      <c r="E11" s="74" t="s">
         <v>80</v>
       </c>
       <c r="F11" s="28" t="s">
@@ -3045,7 +3045,7 @@
       <c r="D12" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="107" t="s">
+      <c r="E12" s="74" t="s">
         <v>84</v>
       </c>
       <c r="F12" s="28" t="s">
@@ -3082,7 +3082,7 @@
       <c r="D13" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="107" t="s">
+      <c r="E13" s="74" t="s">
         <v>85</v>
       </c>
       <c r="F13" s="28" t="s">
@@ -3119,7 +3119,7 @@
       <c r="D14" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="E14" s="107" t="s">
+      <c r="E14" s="74" t="s">
         <v>88</v>
       </c>
       <c r="F14" s="28" t="s">
@@ -3156,7 +3156,7 @@
       <c r="D15" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="E15" s="107" t="s">
+      <c r="E15" s="74" t="s">
         <v>91</v>
       </c>
       <c r="F15" s="28" t="s">
@@ -3193,7 +3193,7 @@
       <c r="D16" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="107" t="s">
+      <c r="E16" s="74" t="s">
         <v>95</v>
       </c>
       <c r="F16" s="28" t="s">
@@ -3230,7 +3230,7 @@
       <c r="D17" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="E17" s="107" t="s">
+      <c r="E17" s="74" t="s">
         <v>98</v>
       </c>
       <c r="F17" s="28" t="s">
@@ -3267,7 +3267,7 @@
       <c r="D18" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="E18" s="107" t="s">
+      <c r="E18" s="74" t="s">
         <v>100</v>
       </c>
       <c r="F18" s="28" t="s">
@@ -3304,7 +3304,7 @@
       <c r="D19" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="107" t="s">
+      <c r="E19" s="74" t="s">
         <v>102</v>
       </c>
       <c r="F19" s="28" t="s">
@@ -3490,16 +3490,16 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="74" t="s">
+      <c r="A27" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="75"/>
+      <c r="B27" s="77"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="77"/>
+      <c r="H27" s="77"/>
       <c r="I27" s="37">
         <f>SUM(I4:I26)</f>
         <v>974.25423728813587</v>
@@ -3518,11 +3518,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A27:H27"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="J1:J3"/>
     <mergeCell ref="K1:K3"/>
@@ -3531,6 +3526,11 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A27:H27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3554,13 +3554,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
@@ -3713,8 +3713,8 @@
   </sheetPr>
   <dimension ref="B1:J44"/>
   <sheetViews>
-    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3730,56 +3730,56 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="99"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="101"/>
     </row>
     <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="100"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="102"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="104"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="104"/>
-      <c r="D5" s="105" t="s">
+      <c r="C5" s="106"/>
+      <c r="D5" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="106"/>
+      <c r="E5" s="108"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="103" t="s">
+      <c r="B6" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="104"/>
-      <c r="D6" s="105">
+      <c r="C6" s="106"/>
+      <c r="D6" s="107">
         <v>10405582436</v>
       </c>
-      <c r="E6" s="106"/>
+      <c r="E6" s="108"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="103" t="s">
+      <c r="B7" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="104"/>
-      <c r="D7" s="105" t="s">
+      <c r="C7" s="106"/>
+      <c r="D7" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="106"/>
+      <c r="E7" s="108"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="105" t="s">
+      <c r="C8" s="106"/>
+      <c r="D8" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="106"/>
+      <c r="E8" s="108"/>
     </row>
     <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
@@ -3904,11 +3904,11 @@
     </row>
     <row r="21" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="94" t="s">
+      <c r="B22" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="95"/>
-      <c r="D22" s="96"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="98"/>
     </row>
     <row r="23" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3946,11 +3946,11 @@
     </row>
     <row r="29" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="94" t="s">
+      <c r="B30" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="95"/>
-      <c r="D30" s="96"/>
+      <c r="C30" s="97"/>
+      <c r="D30" s="98"/>
     </row>
     <row r="31" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="32" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4001,11 +4001,11 @@
     </row>
     <row r="38" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="39" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="94" t="s">
+      <c r="B39" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="95"/>
-      <c r="D39" s="96"/>
+      <c r="C39" s="97"/>
+      <c r="D39" s="98"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E41" s="67"/>

</xml_diff>